<commit_message>
Filled out the full chart.  No ready for review.
</commit_message>
<xml_diff>
--- a/Permissions.xlsx
+++ b/Permissions.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matis/Library/Mobile Documents/com~apple~CloudDocs/IdeaProjects/missionout_backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27DC1808-1D07-9947-AE90-C379AB941BE2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66D4100B-6B59-3D41-8A64-D39FDC6ECB4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9460" yWindow="9880" windowWidth="28040" windowHeight="17440" xr2:uid="{428E7216-AB71-5C42-A777-F2CB3948CD3E}"/>
+    <workbookView xWindow="6080" yWindow="11980" windowWidth="28040" windowHeight="17440" xr2:uid="{428E7216-AB71-5C42-A777-F2CB3948CD3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="21">
   <si>
     <t>Editors</t>
   </si>
@@ -88,13 +88,19 @@
   </si>
   <si>
     <t>Write/Create</t>
+  </si>
+  <si>
+    <t>Updated</t>
+  </si>
+  <si>
+    <t>Permissions for People Using the Missionout Software</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -112,6 +118,20 @@
     </font>
     <font>
       <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="16"/>
       <color theme="1"/>
@@ -121,7 +141,40 @@
     </font>
     <font>
       <b/>
-      <sz val="16"/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="24"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -136,7 +189,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -224,33 +277,74 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="15" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -565,150 +659,258 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3524AEF1-6A39-524B-A18C-E3BC4D59C8A7}">
-  <dimension ref="B1:J14"/>
+  <dimension ref="A2:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="22" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="12"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="14" t="s">
+    <row r="2" spans="1:10" s="25" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+      <c r="D2" s="25" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+    </row>
+    <row r="4" spans="1:10" s="2" customFormat="1" ht="24" x14ac:dyDescent="0.3">
+      <c r="B4" s="7"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="I4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="15"/>
-    </row>
-    <row r="3" spans="2:10" s="1" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="16"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17" t="s">
+      <c r="J4" s="22"/>
+    </row>
+    <row r="5" spans="1:10" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.3">
+      <c r="A5" s="6"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17" t="s">
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="17" t="s">
+      <c r="I5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="18"/>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="19" t="s">
+      <c r="J5" s="12"/>
+    </row>
+    <row r="6" spans="1:10" ht="24" x14ac:dyDescent="0.3">
+      <c r="A6" s="5"/>
+      <c r="B6" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C6" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="8"/>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="19" t="s">
+      <c r="D6" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="14" t="str">
+        <f>B6</f>
+        <v>Editors</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="24" x14ac:dyDescent="0.3">
+      <c r="A7" s="5"/>
+      <c r="B7" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="19" t="s">
+      <c r="C7" s="11"/>
+      <c r="D7" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" s="14" t="str">
+        <f t="shared" ref="J7:J9" si="0">B7</f>
+        <v>Users</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="24" x14ac:dyDescent="0.3">
+      <c r="A8" s="5"/>
+      <c r="B8" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-    </row>
-    <row r="7" spans="2:10" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="19" t="s">
+      <c r="C8" s="11"/>
+      <c r="D8" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="J8" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>Signed In</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="24" x14ac:dyDescent="0.3">
+      <c r="A9" s="5"/>
+      <c r="B9" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="17"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="8"/>
-    </row>
-    <row r="8" spans="2:10" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="20"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="11"/>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E11" t="s">
+      <c r="C9" s="11"/>
+      <c r="D9" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="J9" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>Anyomous</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="5"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="21" t="str">
+        <f>D4</f>
+        <v>User Info</v>
+      </c>
+      <c r="E10" s="21" t="str">
+        <f>E4</f>
+        <v>Token</v>
+      </c>
+      <c r="F10" s="21" t="str">
+        <f>F4</f>
+        <v>Team Info</v>
+      </c>
+      <c r="G10" s="21" t="str">
+        <f>G4</f>
+        <v>Mission Info</v>
+      </c>
+      <c r="H10" s="21" t="str">
+        <f>H4</f>
+        <v>Responces</v>
+      </c>
+      <c r="I10" s="21" t="str">
+        <f>I4</f>
+        <v>Pages</v>
+      </c>
+      <c r="J10" s="20"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="24" x14ac:dyDescent="0.3">
+      <c r="B13" s="4">
+        <v>43922</v>
+      </c>
+      <c r="E13" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F13" s="23" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F12" t="s">
+    <row r="14" spans="1:10" ht="24" x14ac:dyDescent="0.3">
+      <c r="F14" s="23" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F13" t="s">
+    <row r="15" spans="1:10" ht="24" x14ac:dyDescent="0.3">
+      <c r="F15" s="23" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F14" t="s">
+    <row r="16" spans="1:10" ht="24" x14ac:dyDescent="0.3">
+      <c r="F16" s="23" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>